<commit_message>
Starter dialogue, dialogue system tweaks
</commit_message>
<xml_diff>
--- a/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
+++ b/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\OneDrive\Desktop\GGJ\GGJ2024\Detective Game\Data\Dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D16A879-36EF-4BDB-AF3E-C4C6F265AD21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131D8E14-AD0B-4978-ABF9-E8CED921F279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A37DAA-5D7D-4AF5-95A2-1B2A48A38484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="29">
   <si>
     <t>Line #</t>
   </si>
@@ -56,14 +56,73 @@
     <t>Context</t>
   </si>
   <si>
-    <t>HvWRUGUNVxGQdwyAiJLqgjWKDdYQXbihANJAtdMqmSBtAvQBiGvKinayRkbR
-SejuSiguxXEjWCxptVwfzjBKXkNnaGAvEkcvrrvqTQEyPGCjJNKhYRygmSi.</t>
-  </si>
-  <si>
     <t>None</t>
   </si>
   <si>
     <t>Nonsense to get 120 character string</t>
+  </si>
+  <si>
+    <t>Detective</t>
+  </si>
+  <si>
+    <t>AtigMDEYpZVFApUVAPNqciSDkTYzgLZyyzbgQEbgMjwLXuwadAcxckUCTmE.</t>
+  </si>
+  <si>
+    <t>Been getting a lot of reports about unusual happenings here.</t>
+  </si>
+  <si>
+    <t>"Big Time Crime Park"...</t>
+  </si>
+  <si>
+    <t>Clicked on park sign</t>
+  </si>
+  <si>
+    <t>prev</t>
+  </si>
+  <si>
+    <t>Unseen</t>
+  </si>
+  <si>
+    <t>Clicked on chalk outline</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Excuse me, have you seen any aliens around?</t>
+  </si>
+  <si>
+    <t>What happened to you then?</t>
+  </si>
+  <si>
+    <t>I see.</t>
+  </si>
+  <si>
+    <t>I... Uh... Fell from a high place. Completely by accident!</t>
+  </si>
+  <si>
+    <t>Could you stay here and keep a lookout for any aliens for me?</t>
+  </si>
+  <si>
+    <t>Thanks!</t>
+  </si>
+  <si>
+    <t>What? Uh, no...</t>
+  </si>
+  <si>
+    <t>I, um, I'm not going anywhere.</t>
+  </si>
+  <si>
+    <t>Henchman</t>
+  </si>
+  <si>
+    <t>Keep it moving, bub.</t>
+  </si>
+  <si>
+    <t>Clicked on henchman</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -538,24 +597,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8886A688-BCD8-4776-93F2-E7342181866A}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8.7265625" style="8"/>
     <col min="2" max="2" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.90625" style="9" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="37.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.90625" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -566,33 +627,297 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="9" t="s">
+      <c r="B9" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="8">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dialogue updates + dialogue system gets random
</commit_message>
<xml_diff>
--- a/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
+++ b/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\OneDrive\Desktop\GGJ\GGJ2024\Detective Game\Data\Dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE69F3BC-56AF-467C-B7B2-F52326832230}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77559D3F-A11F-4484-8A46-9A7C9F0962A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A37DAA-5D7D-4AF5-95A2-1B2A48A38484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="43">
   <si>
     <t>Line #</t>
   </si>
@@ -132,6 +132,39 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>I have a few safety concerns about your park.</t>
+  </si>
+  <si>
+    <t>Your concerns are noted.</t>
+  </si>
+  <si>
+    <t>Bert</t>
+  </si>
+  <si>
+    <t>Excuse me, small child, have you seen any aliens around?</t>
+  </si>
+  <si>
+    <t>Clicked on Bert</t>
+  </si>
+  <si>
+    <t>Haven't seen one, bub. No aliens here. But...</t>
+  </si>
+  <si>
+    <t>I lost one of my "very special balloons". Green one.</t>
+  </si>
+  <si>
+    <t>Find my balloon and I'll make it worth your while.</t>
+  </si>
+  <si>
+    <t>Yo, you found my "special balloon" yet?</t>
+  </si>
+  <si>
+    <t>not has_balloon</t>
+  </si>
+  <si>
+    <t>Not yet.</t>
   </si>
 </sst>
 </file>
@@ -616,11 +649,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8886A688-BCD8-4776-93F2-E7342181866A}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -629,7 +662,8 @@
     <col min="2" max="2" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.453125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="28.90625" style="5" customWidth="1"/>
     <col min="9" max="16384" width="8.7265625" style="1"/>
@@ -977,6 +1011,209 @@
       <c r="A14" s="4">
         <v>12</v>
       </c>
+      <c r="B14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2">
+        <v>-1</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4">
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4">
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4">
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Trying my hardest to get dialogue progression on press (failed)
</commit_message>
<xml_diff>
--- a/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
+++ b/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\OneDrive\Desktop\GGJ\GGJ2024\Detective Game\Data\Dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77559D3F-A11F-4484-8A46-9A7C9F0962A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA8818C-3079-493F-A698-D0ACE9CC8FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A37DAA-5D7D-4AF5-95A2-1B2A48A38484}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="43">
-  <si>
-    <t>Line #</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
   <si>
     <t>Character</t>
   </si>
@@ -165,13 +162,46 @@
   </si>
   <si>
     <t>Not yet.</t>
+  </si>
+  <si>
+    <t>has_balloon</t>
+  </si>
+  <si>
+    <t>Dialogue Name</t>
+  </si>
+  <si>
+    <t>Observed_Sign</t>
+  </si>
+  <si>
+    <t>Hi_Charlie</t>
+  </si>
+  <si>
+    <t>Wait_Charlie</t>
+  </si>
+  <si>
+    <t>Rand_Hench_1</t>
+  </si>
+  <si>
+    <t>Rand_Hench_2</t>
+  </si>
+  <si>
+    <t>Hi_Bert</t>
+  </si>
+  <si>
+    <t>Bert_NoBalloon</t>
+  </si>
+  <si>
+    <t>Bert_HasBalloon</t>
+  </si>
+  <si>
+    <t>Yes! Here it is.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +221,12 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -649,16 +685,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8886A688-BCD8-4776-93F2-E7342181866A}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="4"/>
+    <col min="1" max="1" width="19.90625" style="4" customWidth="1"/>
     <col min="2" max="2" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.453125" style="2" bestFit="1" customWidth="1"/>
@@ -671,551 +707,604 @@
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="4">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="5" t="s">
+      <c r="D4" s="2">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="4">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="4">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="4">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="4">
-        <v>5</v>
+      <c r="A7" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="2">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="4">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D9" s="2">
+        <v>0</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="D8" s="2">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4">
-        <v>7</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4">
-        <v>8</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>20</v>
       </c>
       <c r="D10" s="2">
         <v>-1</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="2">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4">
-        <v>10</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>25</v>
       </c>
       <c r="D13" s="2">
         <v>-1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4">
-        <v>12</v>
+      <c r="A14" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="2">
         <v>-1</v>
       </c>
       <c r="E14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4">
-        <v>13</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="F15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="2">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="C17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="2">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="4">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="F22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="2">
-        <v>0</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="4">
-        <v>15</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="4">
-        <v>16</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4">
-        <v>17</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4">
-        <v>18</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0</v>
-      </c>
-      <c r="E20" s="2" t="s">
+    </row>
+    <row r="23" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4">
-        <v>19</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>13</v>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
A bunch of dialogues
</commit_message>
<xml_diff>
--- a/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
+++ b/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\OneDrive\Desktop\GGJ\GGJ2024\Detective Game\Data\Dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA8818C-3079-493F-A698-D0ACE9CC8FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD977B49-CDE5-44B0-882E-A33763A647D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A37DAA-5D7D-4AF5-95A2-1B2A48A38484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="67">
   <si>
     <t>Character</t>
   </si>
@@ -146,12 +146,6 @@
     <t>Clicked on Bert</t>
   </si>
   <si>
-    <t>Haven't seen one, bub. No aliens here. But...</t>
-  </si>
-  <si>
-    <t>I lost one of my "very special balloons". Green one.</t>
-  </si>
-  <si>
     <t>Find my balloon and I'll make it worth your while.</t>
   </si>
   <si>
@@ -195,6 +189,54 @@
   </si>
   <si>
     <t>Yes! Here it is.</t>
+  </si>
+  <si>
+    <t>[i]Looks both ways[/i]</t>
+  </si>
+  <si>
+    <t>[i]Slips you a twenty[/i]</t>
+  </si>
+  <si>
+    <t>You never saw me. Got it?</t>
+  </si>
+  <si>
+    <t>Bert_WrongBalloon</t>
+  </si>
+  <si>
+    <t>has_redBalloon</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>Sam_Hi</t>
+  </si>
+  <si>
+    <t>Clicked on Sam</t>
+  </si>
+  <si>
+    <t>You're not looking so good...</t>
+  </si>
+  <si>
+    <t>Did the aliens get you?</t>
+  </si>
+  <si>
+    <t>Haven't seen one, bub. No aliens here. Nope. But...</t>
+  </si>
+  <si>
+    <t>I did lose one of my "very special balloons". Green one.</t>
+  </si>
+  <si>
+    <t>Uuuurgh...</t>
+  </si>
+  <si>
+    <t>What's it.. To you?</t>
+  </si>
+  <si>
+    <t>Listen.. get me some human medicine and I'll tell you.</t>
+  </si>
+  <si>
+    <t>What is that? A red herring? No! I lost my green balloon!</t>
   </si>
 </sst>
 </file>
@@ -685,16 +727,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8886A688-BCD8-4776-93F2-E7342181866A}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.90625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="20.90625" style="4" customWidth="1"/>
     <col min="2" max="2" width="11.6328125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.08984375" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.453125" style="2" bestFit="1" customWidth="1"/>
@@ -707,7 +749,7 @@
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>0</v>
@@ -759,7 +801,7 @@
     </row>
     <row r="3" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>7</v>
@@ -785,7 +827,7 @@
     </row>
     <row r="4" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
@@ -811,7 +853,7 @@
     </row>
     <row r="5" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>7</v>
@@ -837,7 +879,7 @@
     </row>
     <row r="6" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>14</v>
@@ -863,7 +905,7 @@
     </row>
     <row r="7" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
@@ -889,7 +931,7 @@
     </row>
     <row r="8" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>14</v>
@@ -915,7 +957,7 @@
     </row>
     <row r="9" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -941,7 +983,7 @@
     </row>
     <row r="10" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
@@ -967,7 +1009,7 @@
     </row>
     <row r="11" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
@@ -993,7 +1035,7 @@
     </row>
     <row r="12" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>7</v>
@@ -1019,7 +1061,7 @@
     </row>
     <row r="13" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>23</v>
@@ -1045,7 +1087,7 @@
     </row>
     <row r="14" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>7</v>
@@ -1071,7 +1113,7 @@
     </row>
     <row r="15" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>23</v>
@@ -1097,7 +1139,7 @@
     </row>
     <row r="16" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
@@ -1123,13 +1165,13 @@
     </row>
     <row r="17" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D17" s="2">
         <v>0</v>
@@ -1149,13 +1191,13 @@
     </row>
     <row r="18" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -1175,13 +1217,13 @@
     </row>
     <row r="19" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1201,13 +1243,13 @@
     </row>
     <row r="20" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -1216,7 +1258,7 @@
         <v>28</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>5</v>
@@ -1227,13 +1269,13 @@
     </row>
     <row r="21" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1253,13 +1295,13 @@
     </row>
     <row r="22" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D22" s="2">
         <v>10</v>
@@ -1268,7 +1310,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>5</v>
@@ -1279,27 +1321,261 @@
     </row>
     <row r="23" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="2">
-        <v>0</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H23" s="5" t="s">
+      <c r="D25" s="2">
+        <v>0</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Bunch of dialogue stuff
</commit_message>
<xml_diff>
--- a/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
+++ b/Detective Game/Data/Dialogues/_DialoguePlanning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josep\OneDrive\Desktop\GGJ\GGJ2024\Detective Game\Data\Dialogues\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDF43F1D-D064-4FB3-B0D0-B8140FDCD1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C73CAD6-3306-4CBF-98A1-582437CFC49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{24A37DAA-5D7D-4AF5-95A2-1B2A48A38484}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="88">
   <si>
     <t>Character</t>
   </si>
@@ -255,6 +255,51 @@
   </si>
   <si>
     <t>Something may be going on related to your work.</t>
+  </si>
+  <si>
+    <t>Ending</t>
+  </si>
+  <si>
+    <t>? ? ?</t>
+  </si>
+  <si>
+    <t>Well Detective, it seems you've gotten yourself in deep.</t>
+  </si>
+  <si>
+    <t>Game end.</t>
+  </si>
+  <si>
+    <t>Who's there?</t>
+  </si>
+  <si>
+    <t>The Alien Mafia sends its regards.</t>
+  </si>
+  <si>
+    <t>There are so many safety violations around this park!</t>
+  </si>
+  <si>
+    <t>Huh? Wait-</t>
+  </si>
+  <si>
+    <t>And I welcome you to our humble tractor beam testing facility.</t>
+  </si>
+  <si>
+    <t>OSHA's got your number, Glibohp.</t>
+  </si>
+  <si>
+    <t>Alien Don</t>
+  </si>
+  <si>
+    <t>The Alien Mafia? Tractor beam testing facility? Wait...</t>
+  </si>
+  <si>
+    <t>The chalk outline then, that was you?</t>
+  </si>
+  <si>
+    <t>Yes, and the xenon balloon smuggler!</t>
+  </si>
+  <si>
+    <t>And after what I've seen today, the Alien Mafia's going down.</t>
   </si>
 </sst>
 </file>
@@ -745,11 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8886A688-BCD8-4776-93F2-E7342181866A}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1675,6 +1720,262 @@
         <v>12</v>
       </c>
     </row>
+    <row r="36" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" s="2">
+        <v>100</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D43" s="2">
+        <v>0</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D44" s="2">
+        <v>0</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="2">
+        <v>0</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D46" s="2">
+        <v>0</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>